<commit_message>
update results spreadsheet with matmul comparison between pytorch and baseline; Plotter script to save plots; update of subcora script
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AEFFD-4BC3-444E-B84D-0E1D8AC0FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA9A59F-F9B7-A045-B3D3-E737E9A6E306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
+    <sheet name="matmul-optimization" sheetId="2" r:id="rId2"/>
+    <sheet name="GCN-comparison" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,48 +38,208 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>dataset name</t>
-  </si>
-  <si>
-    <t>graph count</t>
-  </si>
-  <si>
-    <t>batch size</t>
-  </si>
-  <si>
-    <t>batch count</t>
-  </si>
-  <si>
-    <t>model name</t>
-  </si>
-  <si>
-    <t>run time (avg of 5 trials)</t>
-  </si>
-  <si>
-    <t>avg run time per batch</t>
-  </si>
-  <si>
-    <t>avg run time per graph</t>
-  </si>
-  <si>
-    <t>device</t>
-  </si>
-  <si>
-    <t>ogbg-molhiv</t>
-  </si>
-  <si>
-    <t>gin</t>
-  </si>
-  <si>
-    <t>gin-virtual-node</t>
-  </si>
-  <si>
-    <t>gcn</t>
-  </si>
-  <si>
-    <t>gcn-virtual-node</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+  <si>
+    <t>Python time</t>
+  </si>
+  <si>
+    <t>Soda command</t>
+  </si>
+  <si>
+    <t>Bambu command</t>
+  </si>
+  <si>
+    <t>Bambu output</t>
+  </si>
+  <si>
+    <t>Experiments to show the difference between Python time and FPGA baseline, explaining why there is the need to use optimizations/why it already accelerate but better results can be achieved</t>
+  </si>
+  <si>
+    <t>Matrix1 size</t>
+  </si>
+  <si>
+    <t>Matrix2 size</t>
+  </si>
+  <si>
+    <t>Selected code</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;15x15xf32&gt;, memref&lt;15x16xf32&gt;) outs(%alloc_1 : memref&lt;15x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+	                     soda-opt \
+	                       -soda-outline-bambu-code \
+	                       -soda-extract-arguments-to-xml=using-bare-ptr \
+	                       -soda-generate-bambu-accelcode=no-aa \
+	                       -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+	                       -mlir-print-ir-after-all \
+	                       output/01searched-edited.mlir \
+	                       -o output/04baseline.mlir \
+	                       2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>15x15</t>
+  </si>
+  <si>
+    <t>15x16</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VV
+D --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocat
+ion-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>1.608 μs</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 25697 cycles
+    Number of executions     : 1
+    Average execution        : 25697 cycles
+    Slices                   : 210
+    Luts                     : 932
+    Power                    : 3.1429999999999998
+    Registers                : 683
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.7549999999999999
+    Design slack             : 0.24500000000000011
+    Frequency                : 266.31158455392813
+    AreaxTime                : 89930.763019999984
+    Time                     : 96.492234999999994
+    Tot. Time                : 96.492234999999994</t>
+  </si>
+  <si>
+    <t>30x30</t>
+  </si>
+  <si>
+    <t>30x16</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;30x30xf32&gt;, memref&lt;30x16xf32&gt;) outs(%alloc_1 : memref&lt;30x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t>60x60</t>
+  </si>
+  <si>
+    <t>60x16</t>
+  </si>
+  <si>
+    <t>90x90</t>
+  </si>
+  <si>
+    <t>90x16</t>
+  </si>
+  <si>
+    <t>2.480 μs</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 101792 cycles
+    Number of executions     : 1
+    Average execution        : 101792 cycles
+    Slices                   : 203
+    Luts                     : 925
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4500000000000002
+    Design slack             : 0.54999999999999982
+    Frequency                : 289.85507246376812
+    AreaxTime                : 324843.71999999997
+    Time                     : 351.18239999999997
+    Tot. Time                : 351.18239999999997</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;60x60xf32&gt;, memref&lt;60x16xf32&gt;) outs(%alloc_1 : memref&lt;60x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t>4.554 μs</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;90x90xf32&gt;, memref&lt;90x16xf32&gt;) outs(%alloc_1 : memref&lt;90x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 405182 cycles
+    Number of executions     : 1
+    Average execution        : 405182 cycles
+    Slices                   : 209
+    Luts                     : 928
+    Power                    : 3.1419999999999999
+    Registers                : 681
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.6189999999999998
+    Design slack             : 0.38100000000000023
+    Frequency                : 276.31942525559549
+    AreaxTime                : 1360776.194624
+    Time                     : 1466.353658
+    Tot. Time                : 1466.353658</t>
+  </si>
+  <si>
+    <t>1.733 μs</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 910172 cycles
+    Number of executions     : 1
+    Average execution        : 910172 cycles
+    Slices                   : 214
+    Luts                     : 956
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4609999999999999
+    Design slack             : 0.53900000000000015
+    Frequency                : 288.93383415197923
+    AreaxTime                : 3011500.6591519997
+    Time                     : 3150.1052919999997
+    Tot. Time                : 3150.1052919999997</t>
+  </si>
+  <si>
+    <t>150x150</t>
+  </si>
+  <si>
+    <t>150x16</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;150x150xf32&gt;, memref&lt;150x16xf32&gt;) outs(%alloc_1 : memref&lt;150x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 2524952 cycles
+    Number of executions     : 1
+    Average execution        : 2524952 cycles
+    Slices                   : 213
+    Luts                     : 957
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.5939999999999999
+    Design slack             : 0.40600000000000014
+    Frequency                : 278.24151363383419
+    AreaxTime                : 8684466.3560159989
+    Time                     : 9074.6774879999994
+    Tot. Time                : 9074.6774879999994</t>
+  </si>
+  <si>
+    <t>5.161 μs</t>
+  </si>
+  <si>
+    <t>120x120</t>
+  </si>
+  <si>
+    <t>120x16</t>
   </si>
 </sst>
 </file>
@@ -121,9 +283,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -438,80 +607,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="9" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="98.6640625" customWidth="1"/>
+    <col min="5" max="5" width="66.5" customWidth="1"/>
+    <col min="6" max="6" width="100" customWidth="1"/>
+    <col min="7" max="7" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="5" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chapter 6 and sota images update
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA9A59F-F9B7-A045-B3D3-E737E9A6E306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82348EDA-853C-B448-9290-719FA531A7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="1840" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Python time</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>120x16</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>linalg.matmul ins(%arg0, %3 : memref&lt;120x120xf32&gt;, memref&lt;120x16xf32&gt;) outs(%alloc_1 : memref&lt;120x16xf32&gt;)</t>
+  </si>
+  <si>
+    <t>4.792 μs</t>
   </si>
 </sst>
 </file>
@@ -283,13 +292,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -607,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,12 +629,12 @@
     <col min="7" max="7" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -639,28 +647,27 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="289" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -673,17 +680,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="289" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -696,17 +703,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="289" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -719,17 +726,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="289" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -742,37 +749,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="289" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
update of chapter 6, result spreadsheet and optimization comparison images
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82348EDA-853C-B448-9290-719FA531A7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0929FE92-F075-5248-9D19-BC325C861CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
     <sheet name="matmul-optimization" sheetId="2" r:id="rId2"/>
     <sheet name="GCN-comparison" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="155">
   <si>
     <t>Python time</t>
   </si>
@@ -250,12 +250,566 @@
   <si>
     <t>4.792 μs</t>
   </si>
+  <si>
+    <t xml:space="preserve">Result of experiments to show the impact of the optimizations of unrolling and different channels </t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Estimated Area</t>
+  </si>
+  <si>
+    <t>matmul</t>
+  </si>
+  <si>
+    <t>Optimizations</t>
+  </si>
+  <si>
+    <t>2 channels, baseline</t>
+  </si>
+  <si>
+    <t>32 channels, baseline</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 2</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 2</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 4</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 4</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 8</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 8</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 15</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+2</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 15+2</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+4</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 15+4</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+8</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 15+8</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+16</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 15+16</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u):$(id -g) -v $(pwd):/working_dir --rm agostini01/soda \
+sh -c "export APPIMAGE_EXTRACT_AND_RUN=1 \
+&amp;&amp; env NO_CLEANUP=1 ./bambu-ac_types-clang16.AppImage -v4 --print-dot \
+-lm --soft-float \
+-fno-unroll-loops \
+--compiler=I386_CLANG16  \
+--device=xcu280-2Lfsvh2892-VVD \
+--clock-period=4.5 \
+--experimental-setup=BAMBU-BALANCED-MP \
+--channels-number=2 \
+--memory-allocation-policy=ALL_BRAM \
+--disable-function-proxy \
+--generate-tb=//working_dir/forward_kernel_test.xml \
+--simulate --simulator=VERILATOR \
+--top-fname=forward_kernel \
+//working_dir/input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u):$(id -g) -v $(pwd):/working_dir --rm agostini01/soda \
+sh -c "export APPIMAGE_EXTRACT_AND_RUN=1 \
+&amp;&amp; env NO_CLEANUP=1 ./bambu-ac_types-clang16.AppImage -v4 --print-dot \
+-lm --soft-float \
+-fno-unroll-loops \
+--compiler=I386_CLANG16  \
+--device=xcu280-2Lfsvh2892-VVD \
+--clock-period=4.5 \
+--experimental-setup=BAMBU-BALANCED-MP \
+--channels-number=32 \
+--memory-allocation-policy=NO_BRAM \
+--disable-function-proxy \
+--generate-tb=//working_dir/forward_kernel_test.xml \
+--simulate --simulator=VERILATOR \
+--top-fname=forward_kernel \
+//working_dir/input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>5013+3947</t>
+  </si>
+  <si>
+    <t>5013+4251</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=2" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>5013+7034+1367</t>
+  </si>
+  <si>
+    <t>5013+7642+1367</t>
+  </si>
+  <si>
+    <t>5013+9538+1367</t>
+  </si>
+  <si>
+    <t>(add\forward_kernel\mul)</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=4" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>5013+12753+1367</t>
+  </si>
+  <si>
+    <t>5013+15957+1367</t>
+  </si>
+  <si>
+    <t>5013+21274+1367</t>
+  </si>
+  <si>
+    <t>5013+17016+1367</t>
+  </si>
+  <si>
+    <t>5013+37046+1367</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=15" \
+                                          -affine-loop-unroll="unroll-factor=2" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll=""unroll-factor=8" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=15" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>Parallel ops</t>
+  </si>
+  <si>
+    <t>5013+20884+1367</t>
+  </si>
+  <si>
+    <t>5013+73168+1367</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-factor=15" \
+                                      -affine-loop-unroll="unroll-factor=4" \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>5013+28640+1367</t>
+  </si>
+  <si>
+    <t>5013+140433+1367</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-factor=15" \
+                                      -affine-loop-unroll="unroll-factor=8" \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>5013+44168+1367</t>
+  </si>
+  <si>
+    <t>5013+271538+1367</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-factor=15" \
+                                      -affine-loop-unroll="unroll-factor=16" \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>Verilator error, probably due to out of memory/area</t>
+  </si>
+  <si>
+    <t>Verilator error, probably due to out of memory/area
+Same experiments worked on Tennin with 813 cycles</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>15x17</t>
+  </si>
+  <si>
+    <t>15x18</t>
+  </si>
+  <si>
+    <t>16 channels, baseline</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u):$(id -g) -v $(pwd):/working_dir --rm agostini01/soda \
+sh -c """"export APPIMAGE_EXTRACT_AND_RUN=1 \
+&amp;&amp; env NO_CLEANUP=1 ./bambu-ac_types-clang16.AppImage -v4 --print-dot \
+-lm --soft-float \
+-fno-unroll-loops \
+--compiler=I386_CLANG16  \
+--device=xcu280-2Lfsvh2892-VVD \
+--clock-period=4.5 \
+--experimental-setup=BAMBU-BALANCED-MP \
+--channels-number=16 \
+--memory-allocation-policy=NO_BRAM \
+--disable-function-proxy \
+--generate-tb=//working_dir/forward_kernel_test.xml \
+--simulate --simulator=VERILATOR \
+--top-fname=forward_kernel \
+//working_dir/input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 2</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 4</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 8</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 15</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 15+2</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 15+4</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 15+8</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 15+16</t>
+  </si>
+  <si>
+    <t>5013+70944+1367</t>
+  </si>
+  <si>
+    <t>5013+137800+1367</t>
+  </si>
+  <si>
+    <t>5013+269301+1367</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=30" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+2</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30+2</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30+2</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+4</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30+4</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30+4</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=30" \
+                                          -affine-loop-unroll="unroll-factor=2" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=30" \
+                                          -affine-loop-unroll="unroll-factor=4" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>5013+529712+1367</t>
+  </si>
+  <si>
+    <t>5013+533278+1367</t>
+  </si>
+  <si>
+    <t>5013+3953</t>
+  </si>
+  <si>
+    <t>5013+4257</t>
+  </si>
+  <si>
+    <t>5013+19848+1367</t>
+  </si>
+  <si>
+    <t>5013+71753+1367</t>
+  </si>
+  <si>
+    <t>5013+69730+1367</t>
+  </si>
+  <si>
+    <t>5013+25365+1367</t>
+  </si>
+  <si>
+    <t>5013+137527+1367</t>
+  </si>
+  <si>
+    <t>5013+134459+1367</t>
+  </si>
+  <si>
+    <t>5013+40080+1367</t>
+  </si>
+  <si>
+    <t>5013+267063+1367</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+5</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30+5</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30+5</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=30" \
+                                          -affine-loop-unroll="unroll-factor=5" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>5013+264185+1367</t>
+  </si>
+  <si>
+    <t>5013+79980+1367</t>
+  </si>
+  <si>
+    <t>5013+325218+1367</t>
+  </si>
+  <si>
+    <t>5013+322419+1367</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=30" \
+                                          -affine-loop-unroll="unroll-factor=16" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+16</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30+16</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30+16</t>
+  </si>
+  <si>
+    <t>5013+260603+1367</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Verilator error</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+8</t>
+  </si>
+  <si>
+    <t>16 channels, unrolling 30+8</t>
+  </si>
+  <si>
+    <t>32 channels, unrolling 30+8</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                        soda-opt \
+                                          -soda-outline-bambu-code \
+                                          -soda-extract-arguments-to-xml=using-bare-ptr \
+                                          -soda-generate-bambu-accelcode \
+                                          -convert-linalg-to-affine-loops \
+                                          -affine-loop-unroll="unroll-factor=30" \
+                                          -affine-loop-unroll="unroll-factor=8" \
+                                          -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                          -mlir-print-ir-after-all \
+                                          output/01searched-edited.mlir \
+                                          -o output/04baseline.mlir \
+                                          2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>5013+521661+1367</t>
+  </si>
+  <si>
+    <t>5013+518224+1367</t>
+  </si>
+  <si>
+    <t>5013+54915+1367</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +821,35 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -292,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -300,6 +883,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,16 +1219,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.6640625" customWidth="1"/>
-    <col min="5" max="5" width="66.5" customWidth="1"/>
-    <col min="6" max="6" width="100" customWidth="1"/>
-    <col min="7" max="7" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -634,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -653,11 +1257,11 @@
       <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -680,7 +1284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -703,7 +1307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -726,7 +1330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -749,7 +1353,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -770,7 +1374,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -800,12 +1404,1574 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="9" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I2" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="6">
+        <v>25697</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <f>15*16*15</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="6">
+        <v>29297</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="6">
+        <f>120/M4*100</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="6">
+        <v>29297</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="6">
+        <v>21152</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="6">
+        <f>2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="6">
+        <v>25007</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="6">
+        <f>2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="6">
+        <v>25007</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="6">
+        <f>2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="6">
+        <v>19457</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="6">
+        <f>4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="6">
+        <v>21857</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="6">
+        <f>4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="6">
+        <v>21857</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="6">
+        <f>4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="6">
+        <v>22637</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="6">
+        <f>8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="6">
+        <v>24767</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="6">
+        <f>8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="6">
+        <v>24767</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="6">
+        <f>8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="6">
+        <v>12377</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="6">
+        <f>15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="6">
+        <v>12767</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="6">
+        <f>15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="6">
+        <v>12767</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="6">
+        <f>15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="6">
+        <v>6257</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="6">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6527</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="6">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="6">
+        <v>6407</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="6">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="6">
+        <v>3317</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" s="6">
+        <f>15*4</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="6">
+        <v>3527</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J23" s="6">
+        <f>15*4</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="10">
+        <v>3287</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J24" s="6">
+        <f>15*4</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="6">
+        <v>2297</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" s="6">
+        <f>15*8</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="10">
+        <v>2027</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="6">
+        <f>15*8</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1787</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="6">
+        <f>15*8</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="6">
+        <f>15*16</f>
+        <v>240</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="6">
+        <v>842</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="6">
+        <f>15*16</f>
+        <v>240</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="6">
+        <v>813</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J30" s="6">
+        <f>15*16</f>
+        <v>240</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" s="6">
+        <v>101792</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J33" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="6">
+        <f>30*16*30</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="6">
+        <v>116192</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J34" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="6">
+        <f>M33*0.01666</f>
+        <v>239.90400000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="6">
+        <v>116192</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J35" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="6">
+        <v>46562</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J36" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="6">
+        <v>47672</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="6">
+        <v>47132</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" s="6">
+        <v>23522</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="6">
+        <v>24872</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J40" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="6">
+        <v>23852</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J41" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" s="6">
+        <v>12242</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J42" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H43" s="6">
+        <v>13472</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J43" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="6">
+        <v>12452</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J44" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45" s="6">
+        <v>45437</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="J45" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="6">
+        <v>47256</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J46" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" s="6">
+        <v>46294</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J47" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H48" s="6">
+        <v>8402</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="J48" s="6">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" s="6">
+        <v>7772</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J49" s="6">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" s="6">
+        <v>6752</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J50" s="6">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H51" s="6">
+        <v>3422</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J51" s="6">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J52" s="6">
+        <v>480</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J53" s="6">
+        <v>480</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update of GCN inference benchmark and results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0929FE92-F075-5248-9D19-BC325C861CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68599A3-6127-7840-9D87-6C77E48D5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="170">
   <si>
     <t>Python time</t>
   </si>
@@ -536,9 +536,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>15x17</t>
-  </si>
-  <si>
     <t>15x18</t>
   </si>
   <si>
@@ -803,6 +800,54 @@
   </si>
   <si>
     <t>5013+54915+1367</t>
+  </si>
+  <si>
+    <t>GCN forward</t>
+  </si>
+  <si>
+    <t>Cora size</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Trade-off min</t>
+  </si>
+  <si>
+    <t>Runtime (s)</t>
+  </si>
+  <si>
+    <t>PyTorch time (s)</t>
+  </si>
+  <si>
+    <t>Mem channels</t>
+  </si>
+  <si>
+    <t>Unroll fact</t>
+  </si>
+  <si>
+    <t>Results of experiments to show that the evaluated optimizations allow to achieve a constant speedup wrt the high-level framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PyTorch time measured using pytorch benchmark, average of 1mln executions </t>
+  </si>
+  <si>
+    <t>59.25 us</t>
+  </si>
+  <si>
+    <t>66.42 us</t>
+  </si>
+  <si>
+    <t>66.75 us</t>
+  </si>
+  <si>
+    <t>88.88 us</t>
+  </si>
+  <si>
+    <t>98.32 us</t>
+  </si>
+  <si>
+    <t>115.03 us</t>
   </si>
 </sst>
 </file>
@@ -849,7 +894,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1220,7 +1265,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1462,10 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="9" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -1465,7 +1513,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
@@ -1500,25 +1548,25 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="6">
         <v>29297</v>
@@ -1531,11 +1579,11 @@
         <v>1</v>
       </c>
       <c r="M5" s="6">
-        <f>120/M4*100</f>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <f>2*SQRT(M4)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
@@ -1566,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
@@ -1597,7 +1645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -1609,13 +1657,13 @@
         <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" s="6">
         <v>25007</v>
@@ -1628,7 +1676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
@@ -1659,7 +1707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>43</v>
       </c>
@@ -1690,7 +1738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
@@ -1702,13 +1750,13 @@
         <v>11</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="6">
         <v>21857</v>
@@ -1721,7 +1769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
@@ -1752,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -1783,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
@@ -1795,13 +1843,13 @@
         <v>11</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="6">
         <v>24767</v>
@@ -1814,7 +1862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1845,7 +1893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>43</v>
       </c>
@@ -1876,7 +1924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -1888,13 +1936,13 @@
         <v>11</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>80</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="6">
         <v>12767</v>
@@ -1907,7 +1955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>43</v>
       </c>
@@ -1938,7 +1986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1969,7 +2017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
@@ -1981,26 +2029,26 @@
         <v>11</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>78</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="6">
         <v>6527</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J20" s="6">
         <f>15*2</f>
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>43</v>
       </c>
@@ -2031,7 +2079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>43</v>
       </c>
@@ -2062,7 +2110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
@@ -2074,26 +2122,26 @@
         <v>11</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H23" s="6">
         <v>3527</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J23" s="6">
         <f>15*4</f>
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
@@ -2124,7 +2172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>43</v>
       </c>
@@ -2155,7 +2203,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>43</v>
       </c>
@@ -2167,26 +2215,26 @@
         <v>11</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>87</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H26" s="10">
         <v>2027</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J26" s="6">
         <f>15*8</f>
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>43</v>
       </c>
@@ -2217,7 +2265,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>43</v>
       </c>
@@ -2238,10 +2286,10 @@
         <v>63</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J28" s="6">
         <f>15*16</f>
@@ -2251,7 +2299,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>43</v>
       </c>
@@ -2263,19 +2311,19 @@
         <v>11</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H29" s="6">
         <v>842</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J29" s="6">
         <f>15*16</f>
@@ -2283,7 +2331,7 @@
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>43</v>
       </c>
@@ -2307,7 +2355,7 @@
         <v>813</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J30" s="6">
         <f>15*16</f>
@@ -2316,8 +2364,9 @@
       <c r="K30" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L30" s="7"/>
+    </row>
+    <row r="33" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>43</v>
       </c>
@@ -2341,7 +2390,7 @@
         <v>101792</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J33" s="6">
         <f>1</f>
@@ -2352,7 +2401,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>43</v>
       </c>
@@ -2364,30 +2413,30 @@
         <v>16</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34" s="6">
         <v>116192</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J34" s="6">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="M34" s="6">
-        <f>M33*0.01666</f>
-        <v>239.90400000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <f>2*SQRT(M33)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>43</v>
       </c>
@@ -2411,14 +2460,14 @@
         <v>116192</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J35" s="6">
         <f>1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>43</v>
       </c>
@@ -2430,10 +2479,10 @@
         <v>16</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>63</v>
@@ -2442,13 +2491,13 @@
         <v>46562</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J36" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>43</v>
       </c>
@@ -2460,25 +2509,25 @@
         <v>16</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H37" s="6">
         <v>47672</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J37" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>43</v>
       </c>
@@ -2490,10 +2539,10 @@
         <v>16</v>
       </c>
       <c r="E38" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>64</v>
@@ -2502,13 +2551,13 @@
         <v>47132</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J38" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>43</v>
       </c>
@@ -2520,10 +2569,10 @@
         <v>16</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>63</v>
@@ -2532,13 +2581,13 @@
         <v>23522</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J39" s="6">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>43</v>
       </c>
@@ -2550,25 +2599,25 @@
         <v>16</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H40" s="6">
         <v>24872</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J40" s="6">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>43</v>
       </c>
@@ -2580,10 +2629,10 @@
         <v>16</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>64</v>
@@ -2592,13 +2641,13 @@
         <v>23852</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J41" s="6">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>43</v>
       </c>
@@ -2610,10 +2659,10 @@
         <v>16</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>63</v>
@@ -2622,13 +2671,13 @@
         <v>12242</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J42" s="6">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -2640,25 +2689,25 @@
         <v>16</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H43" s="6">
         <v>13472</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J43" s="6">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
@@ -2670,10 +2719,10 @@
         <v>16</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>64</v>
@@ -2682,13 +2731,13 @@
         <v>12452</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J44" s="6">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
@@ -2700,10 +2749,10 @@
         <v>16</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>63</v>
@@ -2712,13 +2761,13 @@
         <v>45437</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J45" s="6">
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>43</v>
       </c>
@@ -2730,25 +2779,25 @@
         <v>16</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H46" s="6">
         <v>47256</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J46" s="6">
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>43</v>
       </c>
@@ -2760,10 +2809,10 @@
         <v>16</v>
       </c>
       <c r="E47" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>64</v>
@@ -2772,13 +2821,13 @@
         <v>46294</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J47" s="6">
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>43</v>
       </c>
@@ -2790,10 +2839,10 @@
         <v>16</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>63</v>
@@ -2802,17 +2851,17 @@
         <v>8402</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J48" s="6">
         <f>30*8</f>
         <v>240</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>43</v>
       </c>
@@ -2824,26 +2873,26 @@
         <v>16</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H49" s="6">
         <v>7772</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J49" s="6">
         <f>30*8</f>
         <v>240</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>43</v>
       </c>
@@ -2855,10 +2904,10 @@
         <v>16</v>
       </c>
       <c r="E50" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>64</v>
@@ -2867,14 +2916,14 @@
         <v>6752</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J50" s="6">
         <f>30*8</f>
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>43</v>
       </c>
@@ -2886,10 +2935,10 @@
         <v>16</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>63</v>
@@ -2898,13 +2947,13 @@
         <v>3422</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J51" s="6">
         <v>480</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>43</v>
       </c>
@@ -2916,28 +2965,28 @@
         <v>16</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J52" s="6">
         <v>480</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="6" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>43</v>
       </c>
@@ -2949,25 +2998,25 @@
         <v>16</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>64</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J53" s="6">
         <v>480</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2978,12 +3027,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <f>2*SQRT(C3*16*C3)</f>
+        <v>120</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <f>C3*8</f>
+        <v>120</v>
+      </c>
+      <c r="O3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="0">2*SQRT(C4*16*C4)</f>
+        <v>240</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="1">C4*8</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>720</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7">
+        <v>120</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="E8">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update of plotter script for GCN forward comparison graph
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68599A3-6127-7840-9D87-6C77E48D5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD6E5FF-4885-0549-8306-B668231D0D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added future developments to chapter 7
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5172B73B-BFD0-664B-92C3-6B2341A3F7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3A752-9C63-A942-B9D5-0F8C00C0EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
thesis abstract in italian, results and plotter update
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3A752-9C63-A942-B9D5-0F8C00C0EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0792D1FE-49CD-F64C-B6FE-163130D705D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2120" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="1840" yWindow="2100" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="176">
   <si>
     <t>Python time</t>
   </si>
@@ -823,9 +823,6 @@
     <t>Mem channels</t>
   </si>
   <si>
-    <t>Unroll fact</t>
-  </si>
-  <si>
     <t>Results of experiments to show that the evaluated optimizations allow to achieve a constant speedup wrt the high-level framework</t>
   </si>
   <si>
@@ -848,6 +845,56 @@
   </si>
   <si>
     <t>69.75 us</t>
+  </si>
+  <si>
+    <t>Starting execution of HLS::Evaluation
+    Total cycles             : 1616762 cycles
+    Number of executions     : 1
+    Average execution        : 1616762 cycles
+    Slices                   : 204
+    Luts                     : 926
+    Power                    : 3.1429999999999998
+    Registers                : 680
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4790000000000001
+    Design slack             : 0.52099999999999991
+    Frequency                : 287.43891922966367
+    AreaxTime                : 5208486.0881480007
+    Time                     : 5624.7149980000004
+    Tot. Time                : 5624.7149980000004</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-factor=15" \
+                                      -affine-loop-unroll="unroll-factor=16" \
+                                      -affine-loop-tile \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>Opts</t>
+  </si>
+  <si>
+    <t>Full unroll 2</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1312,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1464,9 @@
       <c r="F8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1435,7 +1484,7 @@
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1451,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,7 +1579,7 @@
       <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="H4" s="6">
@@ -1752,7 +1801,7 @@
       <c r="E11" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -3027,10 +3076,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3049,7 +3098,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3069,7 +3118,7 @@
         <v>160</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>1</v>
@@ -3096,12 +3145,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -3113,20 +3162,25 @@
       <c r="E3">
         <v>32</v>
       </c>
-      <c r="F3">
-        <f>C3*8</f>
-        <v>120</v>
+      <c r="F3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="O3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3138,17 +3192,13 @@
       <c r="E4">
         <v>32</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F8" si="1">C4*8</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5">
         <v>60</v>
@@ -3160,17 +3210,13 @@
       <c r="E5">
         <v>32</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6">
         <v>90</v>
@@ -3182,17 +3228,13 @@
       <c r="E6">
         <v>32</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7">
         <v>120</v>
@@ -3204,17 +3246,13 @@
       <c r="E7">
         <v>32</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8">
         <v>150</v>
@@ -3226,9 +3264,146 @@
       <c r="E8">
         <v>32</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>1200</v>
+    </row>
+    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J12">
+        <v>114345</v>
+      </c>
+      <c r="O12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>174</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13">
+        <v>385650</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J14">
+        <v>1402380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15">
+        <v>3050910</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16">
+        <v>5331240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17">
+        <v>8243370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of thesis introduction and executive summary
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0792D1FE-49CD-F64C-B6FE-163130D705D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B15276-78E6-364B-A31B-A6231C865389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="2100" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="180">
   <si>
     <t>Python time</t>
   </si>
@@ -869,14 +869,28 @@
     <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
   </si>
   <si>
+    <t>Opts</t>
+  </si>
+  <si>
+    <t>Full unroll 2</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>Full unroll 1</t>
+  </si>
+  <si>
     <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
                                     soda-opt \
                                       -soda-outline-bambu-code \
                                       -soda-extract-arguments-to-xml=using-bare-ptr \
                                       -soda-generate-bambu-accelcode \
                                       -convert-linalg-to-affine-loops \
-                                      -affine-loop-unroll="unroll-factor=15" \
-                                      -affine-loop-unroll="unroll-factor=16" \
+                                      -affine-loop-unroll="unroll-full" \
                                       -affine-loop-tile \
                                       -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
                                       -mlir-print-ir-after-all \
@@ -885,16 +899,26 @@
                                       2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
   </si>
   <si>
-    <t>Opts</t>
-  </si>
-  <si>
-    <t>Full unroll 2</t>
-  </si>
-  <si>
-    <t>baseline</t>
-  </si>
-  <si>
-    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+    <t>Experiments with 2 channels and full unroll 1 to see time and area difference wrt 32 channels and full unroll 2</t>
+  </si>
+  <si>
+    <t>Baseline experiments only for number of cycles to create a table showing the difference with the two above computed optimized accelerators</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-full" \
+                                      -affine-loop-unroll="unroll-full" \
+                                      -affine-loop-tile \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
   </si>
 </sst>
 </file>
@@ -3076,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3118,7 +3142,7 @@
         <v>160</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>1</v>
@@ -3163,10 +3187,10 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>170</v>
@@ -3192,6 +3216,15 @@
       <c r="E4">
         <v>32</v>
       </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3210,6 +3243,15 @@
       <c r="E5">
         <v>32</v>
       </c>
+      <c r="F5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3228,6 +3270,15 @@
       <c r="E6">
         <v>32</v>
       </c>
+      <c r="F6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3246,6 +3297,15 @@
       <c r="E7">
         <v>32</v>
       </c>
+      <c r="F7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3264,31 +3324,77 @@
       <c r="E8">
         <v>32</v>
       </c>
+      <c r="F8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>154</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J12">
-        <v>114345</v>
-      </c>
-      <c r="O12" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3296,22 +3402,19 @@
         <v>154</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J13">
-        <v>385650</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3319,22 +3422,19 @@
         <v>154</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J14">
-        <v>1402380</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3342,67 +3442,159 @@
         <v>154</v>
       </c>
       <c r="C15">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J15">
-        <v>3050910</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16">
-        <v>120</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J16">
-        <v>5331240</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>154</v>
       </c>
       <c r="C17">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J17">
+        <v>114345</v>
+      </c>
+      <c r="O17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18">
+        <v>385650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19">
+        <v>1402380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20">
+        <v>90</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20">
+        <v>3050910</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21">
+        <v>120</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>173</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21">
+        <v>5331240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22">
+        <v>150</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J22">
         <v>8243370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update of results and experiments chapter
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B15276-78E6-364B-A31B-A6231C865389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219BEE2-2F26-C443-8E1A-C714ADFB72DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1840" yWindow="2100" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="200">
   <si>
     <t>Python time</t>
   </si>
@@ -811,16 +811,10 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Trade-off min</t>
-  </si>
-  <si>
     <t>Runtime (s)</t>
   </si>
   <si>
     <t>PyTorch time (s)</t>
-  </si>
-  <si>
-    <t>Mem channels</t>
   </si>
   <si>
     <t>Results of experiments to show that the evaluated optimizations allow to achieve a constant speedup wrt the high-level framework</t>
@@ -884,21 +878,6 @@
     <t>Full unroll 1</t>
   </si>
   <si>
-    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
-                                    soda-opt \
-                                      -soda-outline-bambu-code \
-                                      -soda-extract-arguments-to-xml=using-bare-ptr \
-                                      -soda-generate-bambu-accelcode \
-                                      -convert-linalg-to-affine-loops \
-                                      -affine-loop-unroll="unroll-full" \
-                                      -affine-loop-tile \
-                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
-                                      -mlir-print-ir-after-all \
-                                      output/01searched-edited.mlir \
-                                      -o output/04baseline.mlir \
-                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
-  </si>
-  <si>
     <t>Experiments with 2 channels and full unroll 1 to see time and area difference wrt 32 channels and full unroll 2</t>
   </si>
   <si>
@@ -919,6 +898,206 @@
                                       output/01searched-edited.mlir \
                                       -o output/04baseline.mlir \
                                       2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                    soda-opt \
+                                      -soda-outline-bambu-code \
+                                      -soda-extract-arguments-to-xml=using-bare-ptr \
+                                      -soda-generate-bambu-accelcode \
+                                      -convert-linalg-to-affine-loops \
+                                      -affine-loop-unroll="unroll-full" \
+                                      -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                      -mlir-print-ir-after-all \
+                                      output/01searched-edited.mlir \
+                                      -o output/04baseline.mlir \
+                                      2&gt;&amp;1 | cat &gt; output/05intermediate-baseline.mlir</t>
+  </si>
+  <si>
+    <t>Mem chs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 94904 cycles
+    Number of executions     : 1
+    Average execution        : 94904 cycles
+    Slices                   : 28274
+    Luts                     : 118722
+    Power                    : 7.1970000000000001
+    Registers                : 142113
+    DSPs                     : 494
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 8.7989999999999995
+    Design slack             : -4.7989999999999995
+    Frequency                : 113.64927832708263
+    AreaxTime                : 99140028.461712003
+    Time                     : 835.06029599999999
+    Tot. Time                : 835.06029599999999</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --parallel-backend --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>Experiments with 2 channels and full unroll 2 to see if the number of cycles is larger or smaller wrt 32 channels, to see if the tradeoff is won</t>
+  </si>
+  <si>
+    <t>Since evaluating the setting with 32 channels and full unroll 2 seems to be unfeasible, the idea is to use 2 channels with full unrolls 2, showing that the accelerator is faster and speedup does not decrease, and showing difference of number of cycles between the 3 sections below</t>
+  </si>
+  <si>
+    <t>Starting RTL Elaboration : Time (s): cpu = 00:00:06 ; elapsed = 00:00:07 . Memory (MB): peak = 3935.730 ; gain = 491.066 ; free physical = 108233 ; free virtual = 182364
+---------------------------------------------------------------------------------
+INFO: [Synth 8-6157] synthesizing module 'forward_kernel' [/data2/home/demasi/experiments/gcn-inference/cora30/forward_kernel.v:1418360]
+INFO: [Synth 8-6157] synthesizing module '_forward_kernel' [/data2/home/demasi/experiments/gcn-inference/cora30/forward_kernel.v:1241336]
+INFO: [Synth 8-6157] synthesizing module 'controller_forward_kernel' [/data2/home/demasi/experiments/gcn-inference/cora30/forward_kernel.v:564767]
+/opt/Xilinx/Vivado/2021.1/bin/rdiArgs.sh: line 312: 2443397 Killed                  "$RDI_PROG" "$@"
+Parent process (pid 2443397) has died. This helper process will now exit
+error -&gt; Returned error code!
+Please report bugs to &lt;panda-info@polimi.it&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 3987840 cycles
+    Number of executions     : 1
+    Average execution        : 3987840 cycles
+    Slices                   : 43187
+    Luts                     : 218178
+    Power                    : 6.0679999999999996
+    Registers                : 135961
+    DSPs                     : 254
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 7.4350000000000005
+    Design slack             : -3.4350000000000005
+    Frequency                : 134.49899125756556
+    AreaxTime                : 6468888334.2912006
+    Time                     : 29649.590400000001
+    Tot. Time                : 29649.590400000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 93705 cycles
+    Number of executions     : 1
+    Average execution        : 93705 cycles
+    Slices                   : 8338
+    Luts                     : 36265
+    Power                    : 4.25
+    Registers                : 35164
+    DSPs                     : 44
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 5.5839999999999996
+    Design slack             : -1.5839999999999996
+    Frequency                : 179.08309455587394
+    AreaxTime                : 18975614.830799997
+    Time                     : 523.24871999999993
+    Tot. Time                : 523.24871999999993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 301800 cycles
+    Number of executions     : 1
+    Average execution        : 301800 cycles
+    Slices                   : 12448
+    Luts                     : 50907
+    Power                    : 4.4779999999999998
+    Registers                : 50558
+    DSPs                     : 74
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 5.9480000000000004
+    Design slack             : -1.9480000000000004
+    Frequency                : 168.12373907195695
+    AreaxTime                : 91383481.504800007
+    Time                     : 1795.1064000000001
+    Tot. Time                : 1795.1064000000001</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 1064580 cycles
+    Number of executions     : 1
+    Average execution        : 1064580 cycles
+    Slices                   : 21726
+    Luts                     : 94025
+    Power                    : 5.0789999999999997
+    Registers                : 77956
+    DSPs                     : 134
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.702
+    Design slack             : -2.702
+    Frequency                : 149.20919128618323
+    AreaxTime                : 670850995.41900003
+    Time                     : 7134.8151600000001
+    Tot. Time                : 7134.8151600000001</t>
+  </si>
+  <si>
+    <t>in stall for 4 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 2298510 cycles
+    Number of executions     : 1
+    Average execution        : 2298510 cycles
+    Slices                   : 32046
+    Luts                     : 154917
+    Power                    : 5.4459999999999997
+    Registers                : 108770
+    DSPs                     : 194
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.4849999999999994
+    Design slack             : -2.4849999999999994
+    Frequency                : 154.20200462606016
+    AreaxTime                : 2309167604.7499499
+    Time                     : 14905.837349999998
+    Tot. Time                : 14905.837349999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 6136470 cycles
+    Number of executions     : 1
+    Average execution        : 6136470 cycles
+    Slices                   : 27002
+    Luts                     : 115463
+    Power                    : 6.335
+    Registers                : 143916
+    DSPs                     : 26
+    BRAMs                    : 264
+    Clock period             : 4
+    Design minimum period    : 6.702
+    Design slack             : -2.702
+    Frequency                : 149.20919128618323
+    AreaxTime                : 4748603149.0582199
+    Time                     : 41126.621939999997
+    Tot. Time                : 41126.621939999997</t>
+  </si>
+  <si>
+    <t>523.24 ns</t>
+  </si>
+  <si>
+    <t>1.79 us</t>
+  </si>
+  <si>
+    <t>7.13 us</t>
+  </si>
+  <si>
+    <t>14.90 us</t>
+  </si>
+  <si>
+    <t>29.64 us</t>
+  </si>
+  <si>
+    <t>41.12 us</t>
+  </si>
+  <si>
+    <t>Errors</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1019,6 +1198,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1336,7 +1516,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1669,7 @@
         <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1525,7 +1705,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,7 +1763,7 @@
         <v>81</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3100,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3111,490 +3291,657 @@
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <f>2*SQRT(C3*16*C3)</f>
-        <v>120</v>
-      </c>
-      <c r="E3">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="O3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>154</v>
       </c>
-      <c r="B4" t="s">
-        <v>164</v>
-      </c>
       <c r="C4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D8" si="0">2*SQRT(C4*16*C4)</f>
-        <v>240</v>
-      </c>
-      <c r="E4">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
-        <v>172</v>
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>154</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C5">
-        <v>60</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-      <c r="E5">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>154</v>
       </c>
-      <c r="B6" t="s">
-        <v>165</v>
-      </c>
       <c r="C6">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>720</v>
-      </c>
-      <c r="E6">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
-        <v>172</v>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>154</v>
       </c>
-      <c r="B7" t="s">
-        <v>166</v>
-      </c>
       <c r="C7">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>960</v>
-      </c>
-      <c r="E7">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
-        <v>172</v>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>154</v>
       </c>
-      <c r="B8" t="s">
-        <v>167</v>
-      </c>
       <c r="C8">
+        <v>120</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9">
         <v>150</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E8">
+      <c r="D9">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="E9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>175</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="O10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>154</v>
       </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
       <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>175</v>
+      <c r="E11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11">
+        <v>93705</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="M11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>154</v>
       </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
       <c r="C12">
-        <v>60</v>
-      </c>
-      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
-        <v>175</v>
+      <c r="E12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="H12" t="s">
+        <v>194</v>
+      </c>
+      <c r="I12">
+        <v>301800</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
       <c r="C13">
-        <v>90</v>
-      </c>
-      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="F13" t="s">
-        <v>175</v>
+      <c r="E13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="H13" t="s">
+        <v>195</v>
+      </c>
+      <c r="I13">
+        <v>1064580</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
+      <c r="B14" t="s">
+        <v>163</v>
+      </c>
       <c r="C14">
-        <v>120</v>
-      </c>
-      <c r="E14">
+        <v>90</v>
+      </c>
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="F14" t="s">
-        <v>175</v>
+      <c r="E14" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="H14" t="s">
+        <v>196</v>
+      </c>
+      <c r="I14">
+        <v>2298510</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>154</v>
       </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
       <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" t="s">
+        <v>197</v>
+      </c>
+      <c r="I15">
+        <v>3987840</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16">
         <v>150</v>
       </c>
-      <c r="E15">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E16" t="s">
         <v>173</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J17">
-        <v>114345</v>
-      </c>
-      <c r="O17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H16" t="s">
+        <v>198</v>
+      </c>
+      <c r="I16">
+        <v>6136470</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>154</v>
       </c>
       <c r="C18">
-        <v>30</v>
-      </c>
-      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
+      <c r="E18" t="s">
+        <v>170</v>
+      </c>
       <c r="F18" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J18">
-        <v>385650</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+      <c r="M18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>154</v>
       </c>
       <c r="C19">
-        <v>60</v>
-      </c>
-      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19" t="s">
+        <v>170</v>
+      </c>
       <c r="F19" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J19">
-        <v>1402380</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>154</v>
       </c>
       <c r="C20">
-        <v>90</v>
-      </c>
-      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="D20">
         <v>2</v>
       </c>
+      <c r="E20" t="s">
+        <v>170</v>
+      </c>
       <c r="F20" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J20">
-        <v>3050910</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>154</v>
       </c>
       <c r="C21">
-        <v>120</v>
-      </c>
-      <c r="E21">
+        <v>90</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
+      <c r="E21" t="s">
+        <v>170</v>
+      </c>
       <c r="F21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J21">
-        <v>5331240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>154</v>
       </c>
       <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23">
         <v>150</v>
       </c>
-      <c r="E22">
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="E23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J22">
+      <c r="G25" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25">
+        <v>114345</v>
+      </c>
+      <c r="M25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26">
+        <v>385650</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27">
+        <v>1402380</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28">
+        <v>3050910</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29">
+        <v>120</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29">
+        <v>5331240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30">
+        <v>150</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30">
         <v>8243370</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update of results and experiments chapter with plotters
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219BEE2-2F26-C443-8E1A-C714ADFB72DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E34ED45-9E43-814E-AD3F-9768406C275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2100" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="1160" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="204">
   <si>
     <t>Python time</t>
   </si>
@@ -860,9 +860,6 @@
     Tot. Time                : 5624.7149980000004</t>
   </si>
   <si>
-    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
-  </si>
-  <si>
     <t>Opts</t>
   </si>
   <si>
@@ -870,9 +867,6 @@
   </si>
   <si>
     <t>baseline</t>
-  </si>
-  <si>
-    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
   </si>
   <si>
     <t>Full unroll 1</t>
@@ -936,9 +930,6 @@
     Tot. Time                : 835.06029599999999</t>
   </si>
   <si>
-    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --parallel-backend --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
-  </si>
-  <si>
     <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
   </si>
   <si>
@@ -979,25 +970,6 @@
   </si>
   <si>
     <t xml:space="preserve">  Starting execution of HLS::Evaluation
-    Total cycles             : 93705 cycles
-    Number of executions     : 1
-    Average execution        : 93705 cycles
-    Slices                   : 8338
-    Luts                     : 36265
-    Power                    : 4.25
-    Registers                : 35164
-    DSPs                     : 44
-    BRAMs                    : 256
-    Clock period             : 4
-    Design minimum period    : 5.5839999999999996
-    Design slack             : -1.5839999999999996
-    Frequency                : 179.08309455587394
-    AreaxTime                : 18975614.830799997
-    Time                     : 523.24871999999993
-    Tot. Time                : 523.24871999999993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Starting execution of HLS::Evaluation
     Total cycles             : 301800 cycles
     Number of executions     : 1
     Average execution        : 301800 cycles
@@ -1099,12 +1071,265 @@
   <si>
     <t>Errors</t>
   </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --parallel-backend --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>./bambu-dev-panda.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --parallel-backend --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --parallel-backend --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             : 93705 cycles
+    Number of executions     : 1
+    Average execution        : 93705 cycles
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Slices</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                   : 8338
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Luts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                     : 36265
+    Power                    : 4.25
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Registers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                : 35164
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DSPs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                     : 44
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BRAMs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                    : 256
+    Clock period             : 4
+    Design minimum period    : 5.5839999999999996
+    Design slack             : -1.5839999999999996
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frequency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                : 179.08309455587394
+    AreaxTime                : 18975614.830799997
+    Time                     : 523.24871999999993
+    Tot. Time                : 523.24871999999993</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 5332200 cycles
+    Number of executions     : 1
+    Average execution        : 5332200 cycles
+    Slices                   : 8045
+    Luts                     : 30441
+    Power                    : 4.1299999999999999
+    Registers                : 25878
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.859
+    Design slack             : -2.859
+    Frequency                : 145.79384749963552
+    AreaxTime                : 1113335733.8717999
+    Time                     : 36573.559800000003
+    Tot. Time                : 36573.559800000003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 8244570 cycles
+    Number of executions     : 1
+    Average execution        : 8244570 cycles
+    Slices                   : 7499
+    Luts                     : 29390
+    Power                    : 4.1289999999999996
+    Registers                : 26015
+    DSPs                     : 16
+    BRAMs                    : 264
+    Clock period             : 4
+    Design minimum period    : 6.1120000000000001
+    Design slack             : -2.1120000000000001
+    Frequency                : 163.61256544502618
+    AreaxTime                : 1480985959.9776001
+    Time                     : 50390.811840000002
+    Tot. Time                : 50390.811840000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 115852 cycles
+    Number of executions     : 1
+    Average execution        : 115852 cycles
+    Slices                   : 8307
+    Luts                     : 32927
+    Power                    : 4.1379999999999999
+    Registers                : 32195
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.7669999999999995
+    Design slack             : -2.7669999999999995
+    Frequency                : 147.77597162701346
+    AreaxTime                : 25813796.126667999
+    Time                     : 783.97048399999994
+    Tot. Time                : 783.97048399999994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 385874 cycles
+    Number of executions     : 1
+    Average execution        : 385874 cycles
+    Slices                   : 7457
+    Luts                     : 30379
+    Power                    : 4.1100000000000003
+    Registers                : 26925
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.319
+    Design slack             : -2.319
+    Frequency                : 158.25288811520809
+    AreaxTime                : 74074264.20847401
+    Time                     : 2438.337806
+    Tot. Time                : 2438.337806</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1144,7 +1369,15 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF7030A0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1170,7 +1403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1195,10 +1428,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1705,7 +1941,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1763,7 +1999,7 @@
         <v>81</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2073,7 +2309,7 @@
       <c r="G13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="11">
         <v>22637</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -2104,7 +2340,7 @@
       <c r="G14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="11">
         <v>24767</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -2135,7 +2371,7 @@
       <c r="G15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="11">
         <v>24767</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -2414,7 +2650,7 @@
       <c r="G24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="12">
         <v>3287</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -2476,7 +2712,7 @@
       <c r="G26" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="12">
         <v>2027</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -3010,7 +3246,7 @@
       <c r="G45" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="11">
         <v>45437</v>
       </c>
       <c r="I45" s="6" t="s">
@@ -3040,7 +3276,7 @@
       <c r="G46" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46" s="11">
         <v>47256</v>
       </c>
       <c r="I46" s="6" t="s">
@@ -3070,7 +3306,7 @@
       <c r="G47" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47" s="11">
         <v>46294</v>
       </c>
       <c r="I47" s="6" t="s">
@@ -3134,7 +3370,7 @@
       <c r="G49" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49" s="12">
         <v>7772</v>
       </c>
       <c r="I49" s="6" t="s">
@@ -3165,7 +3401,7 @@
       <c r="G50" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50" s="12">
         <v>6752</v>
       </c>
       <c r="I50" s="6" t="s">
@@ -3282,8 +3518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3306,7 +3542,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3320,10 +3556,10 @@
         <v>155</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
@@ -3344,7 +3580,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>93</v>
@@ -3361,16 +3597,16 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M4" t="s">
         <v>160</v>
@@ -3387,16 +3623,16 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>184</v>
+        <v>197</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3410,16 +3646,16 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>190</v>
+        <v>197</v>
+      </c>
+      <c r="L6" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3433,13 +3669,13 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3453,13 +3689,13 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3473,13 +3709,13 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3496,25 +3732,25 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I11">
         <v>93705</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="M11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3531,22 +3767,22 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I12">
         <v>301800</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3563,22 +3799,22 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I13">
         <v>1064580</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3595,22 +3831,22 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I14">
         <v>2298510</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3627,22 +3863,22 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I15">
         <v>3987840</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3659,22 +3895,22 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="H16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I16">
         <v>6136470</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3692,16 +3928,16 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3715,13 +3951,13 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3735,13 +3971,13 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3755,13 +3991,13 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3775,13 +4011,13 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3795,13 +4031,13 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3815,19 +4051,19 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>171</v>
-      </c>
-      <c r="F25" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25">
-        <v>114345</v>
+        <v>37</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="M25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3841,16 +4077,16 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I26">
-        <v>385650</v>
+        <v>37</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3864,17 +4100,18 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="I27">
         <v>1402380</v>
       </c>
+      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -3887,17 +4124,18 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="I28">
         <v>3050910</v>
       </c>
+      <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -3910,16 +4148,16 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29">
-        <v>5331240</v>
+        <v>37</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3933,20 +4171,21 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I30">
-        <v>8243370</v>
+        <v>37</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update of chapter six
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E34ED45-9E43-814E-AD3F-9768406C275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0811EC70-8269-8448-B433-1F3468FBF945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="206">
   <si>
     <t>Python time</t>
   </si>
@@ -1324,6 +1324,44 @@
     Time                     : 2438.337806
     Tot. Time                : 2438.337806</t>
   </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 3051630 cycles
+    Number of executions     : 1
+    Average execution        : 3051630 cycles
+    Slices                   : 6769
+    Luts                     : 29899
+    Power                    : 4.0730000000000004
+    Registers                : 25966
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 5.9990000000000006
+    Design slack             : -1.9990000000000006
+    Frequency                : 166.69444907484578
+    AreaxTime                : 547352871.53463006
+    Time                     : 18306.728370000004
+    Tot. Time                : 18306.728370000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 1402860 cycles
+    Number of executions     : 1
+    Average execution        : 1402860 cycles
+    Slices                   : 6928
+    Luts                     : 30115
+    Power                    : 4.0629999999999997
+    Registers                : 24287
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.3260000000000005
+    Design slack             : -2.3260000000000005
+    Frequency                : 158.07777426493834
+    AreaxTime                : 267255337.42140001
+    Time                     : 8874.4923600000002
+    Tot. Time                : 8874.4923600000002</t>
+  </si>
 </sst>
 </file>
 
@@ -1403,7 +1441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1428,7 +1466,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2309,7 +2346,7 @@
       <c r="G13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>22637</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -2340,7 +2377,7 @@
       <c r="G14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>24767</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -2371,7 +2408,7 @@
       <c r="G15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>24767</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -2650,7 +2687,7 @@
       <c r="G24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="11">
         <v>3287</v>
       </c>
       <c r="I24" s="6" t="s">
@@ -2712,7 +2749,7 @@
       <c r="G26" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="11">
         <v>2027</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -3246,7 +3283,7 @@
       <c r="G45" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="10">
         <v>45437</v>
       </c>
       <c r="I45" s="6" t="s">
@@ -3276,7 +3313,7 @@
       <c r="G46" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="10">
         <v>47256</v>
       </c>
       <c r="I46" s="6" t="s">
@@ -3306,7 +3343,7 @@
       <c r="G47" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="10">
         <v>46294</v>
       </c>
       <c r="I47" s="6" t="s">
@@ -3370,7 +3407,7 @@
       <c r="G49" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H49" s="12">
+      <c r="H49" s="11">
         <v>7772</v>
       </c>
       <c r="I49" s="6" t="s">
@@ -3401,7 +3438,7 @@
       <c r="G50" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H50" s="12">
+      <c r="H50" s="11">
         <v>6752</v>
       </c>
       <c r="I50" s="6" t="s">
@@ -3519,7 +3556,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3631,7 +3668,7 @@
       <c r="G5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3737,7 +3774,7 @@
       <c r="F11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" t="s">
         <v>198</v>
       </c>
       <c r="H11" t="s">
@@ -3772,7 +3809,7 @@
       <c r="F12" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" t="s">
         <v>198</v>
       </c>
       <c r="H12" t="s">
@@ -3804,7 +3841,7 @@
       <c r="F13" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" t="s">
         <v>198</v>
       </c>
       <c r="H13" t="s">
@@ -3836,7 +3873,7 @@
       <c r="F14" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" t="s">
         <v>198</v>
       </c>
       <c r="H14" t="s">
@@ -3868,7 +3905,7 @@
       <c r="F15" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" t="s">
         <v>198</v>
       </c>
       <c r="H15" t="s">
@@ -3900,7 +3937,7 @@
       <c r="F16" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" t="s">
         <v>198</v>
       </c>
       <c r="H16" t="s">
@@ -4053,7 +4090,7 @@
       <c r="E25" t="s">
         <v>170</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -4108,10 +4145,9 @@
       <c r="G27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I27">
-        <v>1402380</v>
-      </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="4" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -4132,10 +4168,9 @@
       <c r="G28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I28">
-        <v>3050910</v>
-      </c>
-      <c r="K28" s="10"/>
+      <c r="K28" s="4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">

</xml_diff>

<commit_message>
update of results spreadsheet
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0811EC70-8269-8448-B433-1F3468FBF945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B22836-ED97-1040-AF7E-1B6FA10C8D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -3555,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update of chapter six and executive summary
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B22836-ED97-1040-AF7E-1B6FA10C8D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6621BB7-D39C-3349-A10D-F22FEB8BDC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -3556,7 +3556,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
save binary function to export tensor data + results update
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6621BB7-D39C-3349-A10D-F22FEB8BDC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6981A7-B7E3-1D4F-937E-C3AB2F4BE89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="matmul-comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="238">
   <si>
     <t>Python time</t>
   </si>
@@ -1362,6 +1362,311 @@
     Time                     : 8874.4923600000002
     Tot. Time                : 8874.4923600000002</t>
   </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm -fno-unroll-loops --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm -fno-unroll-loops --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>Baseline experiments with -fno-unroll-loops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline experiments with -fno-unroll-loops and NO_BRAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 142320 cycles
+    Number of executions     : 1
+    Average execution        : 142320 cycles
+    Slices                   : 2676
+    Luts                     : 13012
+    Power                    : 3.2770000000000001
+    Registers                : 10253
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.8620000000000001
+    Design slack             : 0.1379999999999999
+    Frequency                : 258.93319523562923
+    AreaxTime                : 7151913.5980799999
+    Time                     : 549.63983999999994
+    Tot. Time                : 549.63983999999994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 385650 cycles
+    Number of executions     : 1
+    Average execution        : 385650 cycles
+    Slices                   : 3498
+    Luts                     : 17177
+    Power                    : 3.6720000000000002
+    Registers                : 9157
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.7119999999999997
+    Design slack             : -2.7119999999999997
+    Frequency                : 148.98688915375448
+    AreaxTime                : 44462369.055599995
+    Time                     : 2588.4827999999998
+    Tot. Time                : 2588.4827999999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 476490 cycles
+    Number of executions     : 1
+    Average execution        : 476490 cycles
+    Slices                   : 2706
+    Luts                     : 13522
+    Power                    : 3.2709999999999999
+    Registers                : 10240
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.8340000000000001
+    Design slack             : 0.16599999999999993
+    Frequency                : 260.82420448617631
+    AreaxTime                : 24702836.888519999
+    Time                     : 1826.86266
+    Tot. Time                : 1826.86266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 114345 cycles
+    Number of executions     : 1
+    Average execution        : 114345 cycles
+    Slices                   : 3827
+    Luts                     : 17131
+    Power                    : 3.6819999999999999
+    Registers                : 9209
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.3339999999999996
+    Design slack             : -2.3339999999999996
+    Frequency                : 157.87811809283235
+    AreaxTime                : 12407319.131129999
+    Time                     : 724.26122999999995
+    Tot. Time                : 724.26122999999995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 1402380 cycles
+    Number of executions     : 1
+    Average execution        : 1402380 cycles
+    Slices                   : 4049
+    Luts                     : 17483
+    Power                    : 3.6779999999999999
+    Registers                : 9228
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.8049999999999997
+    Design slack             : -2.8049999999999997
+    Frequency                : 146.95077149155034
+    AreaxTime                : 166843693.9197
+    Time                     : 9543.1958999999988
+    Tot. Time                : 9543.1958999999988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 1724310 cycles
+    Number of executions     : 1
+    Average execution        : 1724310 cycles
+    Slices                   : 2662
+    Luts                     : 13118
+    Power                    : 3.2869999999999999
+    Registers                : 10239
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.7650000000000001
+    Design slack             : 0.23499999999999988
+    Frequency                : 265.60424966799468
+    AreaxTime                : 85162412.153700009
+    Time                     : 6492.0271499999999
+    Tot. Time                : 6492.0271499999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 3050910 cycles
+    Number of executions     : 1
+    Average execution        : 3050910 cycles
+    Slices                   : 4091
+    Luts                     : 17783
+    Power                    : 3.6869999999999998
+    Registers                : 9182
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.4109999999999996
+    Design slack             : -2.4109999999999996
+    Frequency                : 155.98190609889255
+    AreaxTime                : 347824525.84982997
+    Time                     : 19559.384009999998
+    Tot. Time                : 19559.384009999998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 3744330 cycles
+    Number of executions     : 1
+    Average execution        : 3744330 cycles
+    Slices                   : 2803
+    Luts                     : 13597
+    Power                    : 3.2709999999999999
+    Registers                : 10246
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.9500000000000002
+    Design slack             : 0.049999999999999822
+    Frequency                : 253.1645569620253
+    AreaxTime                : 201101037.2895
+    Time                     : 14790.103500000001
+    Tot. Time                : 14790.103500000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 5331240 cycles
+    Number of executions     : 1
+    Average execution        : 5331240 cycles
+    Slices                   : 4231
+    Luts                     : 17961
+    Power                    : 3.6840000000000002
+    Registers                : 9148
+    DSPs                     : 16
+    BRAMs                    : 256
+    Clock period             : 4
+    Design minimum period    : 6.4619999999999997
+    Design slack             : -2.4619999999999997
+    Frequency                : 154.75085112968122
+    AreaxTime                : 618764943.39767992
+    Time                     : 34450.472880000001
+    Tot. Time                : 34450.472880000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 6536550 cycles
+    Number of executions     : 1
+    Average execution        : 6536550 cycles
+    Slices                   : 2888
+    Luts                     : 13520
+    Power                    : 3.2890000000000001
+    Registers                : 10241
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.819
+    Design slack             : 0.18100000000000005
+    Frequency                : 261.84865147944487
+    AreaxTime                : 337500901.764
+    Time                     : 24963.084450000002
+    Tot. Time                : 24963.084450000002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 8243370 cycles
+    Number of executions     : 1
+    Average execution        : 8243370 cycles
+    Slices                   : 3849
+    Luts                     : 17188
+    Power                    : 3.6800000000000002
+    Registers                : 9163
+    DSPs                     : 16
+    BRAMs                    : 264
+    Clock period             : 4
+    Design minimum period    : 6.2270000000000003
+    Design slack             : -2.2270000000000003
+    Frequency                : 160.59097478721694
+    AreaxTime                : 882285220.24812007
+    Time                     : 51331.464990000008
+    Tot. Time                : 51331.464990000008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 10100970 cycles
+    Number of executions     : 1
+    Average execution        : 10100970 cycles
+    Slices                   : 2786
+    Luts                     : 13685
+    Power                    : 3.2829999999999999
+    Registers                : 10240
+    DSPs                     : 16
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.8650000000000002
+    Design slack             : 0.13499999999999979
+    Frequency                : 258.73221216041395
+    AreaxTime                : 534265808.24925005
+    Time                     : 39040.249050000006
+    Tot. Time                : 39040.249050000006</t>
+  </si>
+  <si>
+    <t>Bambu command (no-unroll)</t>
+  </si>
+  <si>
+    <t>Bambu output (no-unroll)</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VV
+D --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocat
+ion-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>2 channels, baseline, NOBRAM</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u):$(id -g) -v $(pwd):/working_dir --rm agostini01/soda \
+sh -c "export APPIMAGE_EXTRACT_AND_RUN=1 \
+&amp;&amp; env NO_CLEANUP=1 ./bambu-ac_types-clang16.AppImage -v4 --print-dot \
+-lm --soft-float \
+-fno-unroll-loops \
+--compiler=I386_CLANG16  \
+--device=xcu280-2Lfsvh2892-VVD \
+--clock-period=4.5 \
+--experimental-setup=BAMBU-BALANCED-MP \
+--channels-number=2 \
+--memory-allocation-policy=NO_BRAM \
+--disable-function-proxy \
+--generate-tb=//working_dir/forward_kernel_test.xml \
+--simulate --simulator=VERILATOR \
+--top-fname=forward_kernel \
+//working_dir/input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 2, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 4, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 8, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+2, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+4, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 15+8, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+2, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+4, NOBRAM</t>
+  </si>
+  <si>
+    <t>2 channels, unrolling 30+8, NOBRAM</t>
+  </si>
 </sst>
 </file>
 
@@ -1441,7 +1746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1472,6 +1777,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1786,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1802,12 +2108,12 @@
     <col min="7" max="7" width="24" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1829,8 +2135,14 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1852,8 +2164,12 @@
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1875,8 +2191,12 @@
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1898,8 +2218,12 @@
       <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1921,8 +2245,12 @@
       <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1944,8 +2272,12 @@
       <c r="G8" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1967,6 +2299,10 @@
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1975,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3545,6 +3881,279 @@
         <v>146</v>
       </c>
     </row>
+    <row r="57" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3553,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319BDD64-DC34-4D4C-BEED-D9635FFF367C}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3755,6 +4364,11 @@
         <v>197</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
     <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>154</v>
@@ -3783,11 +4397,8 @@
       <c r="I11">
         <v>93705</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="12" t="s">
         <v>199</v>
-      </c>
-      <c r="M11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3818,7 +4429,7 @@
       <c r="I12">
         <v>301800</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="12" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3850,7 +4461,7 @@
       <c r="I13">
         <v>1064580</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="12" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3882,7 +4493,7 @@
       <c r="I14">
         <v>2298510</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="12" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3914,7 +4525,7 @@
       <c r="I15">
         <v>3987840</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="12" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3946,15 +4557,18 @@
       <c r="I16">
         <v>6136470</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3973,11 +4587,8 @@
       <c r="G18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="M18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -3997,7 +4608,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -4017,7 +4628,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -4037,7 +4648,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>154</v>
       </c>
@@ -4057,7 +4668,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -4077,7 +4688,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -4096,14 +4712,11 @@
       <c r="G25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="M25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -4122,11 +4735,11 @@
       <c r="G26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="12" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>154</v>
       </c>
@@ -4145,11 +4758,11 @@
       <c r="G27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="12" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -4168,11 +4781,11 @@
       <c r="G28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>154</v>
       </c>
@@ -4191,11 +4804,11 @@
       <c r="G29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="12" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -4214,8 +4827,295 @@
       <c r="G30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="12" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35">
+        <v>90</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36">
+        <v>120</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37">
+        <v>150</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K38" s="12"/>
+    </row>
+    <row r="39" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>170</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40">
+        <v>30</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41">
+        <v>60</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42">
+        <v>90</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>170</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43">
+        <v>120</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44">
+        <v>150</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[R4] chapter 5/6 first update
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6981A7-B7E3-1D4F-937E-C3AB2F4BE89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D46FC8-B2B6-FA4E-9EF5-8921DC1E8D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="246">
   <si>
     <t>Python time</t>
   </si>
@@ -1603,12 +1603,6 @@
     Tot. Time                : 39040.249050000006</t>
   </si>
   <si>
-    <t>Bambu command (no-unroll)</t>
-  </si>
-  <si>
-    <t>Bambu output (no-unroll)</t>
-  </si>
-  <si>
     <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VV
 D --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocat
 ion-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
@@ -1666,6 +1660,132 @@
   </si>
   <si>
     <t>2 channels, unrolling 30+8, NOBRAM</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v4 --print-dot -lm --soft-float -fno-unroll-loops --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4 --experimental-setup=BAMBU-BALANCED-MP --channels-number=2 --memory-allocation-policy=ALL_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 25697 cycles
+    Number of executions     : 1
+    Average execution        : 25697 cycles
+    Slices                   : 210
+    Luts                     : 932
+    Power                    : 3.1429999999999998
+    Registers                : 683
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.7549999999999999
+    Design slack             : 0.24500000000000011
+    Frequency                : 266.31158455392813
+    AreaxTime                : 89930.763019999984
+    Time                     : 96.492234999999994
+    Tot. Time                : 96.492234999999994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 101792 cycles
+    Number of executions     : 1
+    Average execution        : 101792 cycles
+    Slices                   : 203
+    Luts                     : 925
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4500000000000002
+    Design slack             : 0.54999999999999982
+    Frequency                : 289.85507246376812
+    AreaxTime                : 324843.71999999997
+    Time                     : 351.18239999999997
+    Tot. Time                : 351.18239999999997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 405182 cycles
+    Number of executions     : 1
+    Average execution        : 405182 cycles
+    Slices                   : 209
+    Luts                     : 928
+    Power                    : 3.1419999999999999
+    Registers                : 681
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.6189999999999998
+    Design slack             : 0.38100000000000023
+    Frequency                : 276.31942525559549
+    AreaxTime                : 1360776.194624
+    Time                     : 1466.353658
+    Tot. Time                : 1466.353658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 910172 cycles
+    Number of executions     : 1
+    Average execution        : 910172 cycles
+    Slices                   : 214
+    Luts                     : 956
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4609999999999999
+    Design slack             : 0.53900000000000015
+    Frequency                : 288.93383415197923
+    AreaxTime                : 3011500.6591519997
+    Time                     : 3150.1052919999997
+    Tot. Time                : 3150.1052919999997</t>
+  </si>
+  <si>
+    <t>Bambu command (-fno-unroll)</t>
+  </si>
+  <si>
+    <t>Bambu output (-fno-unroll)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 1616762 cycles
+    Number of executions     : 1
+    Average execution        : 1616762 cycles
+    Slices                   : 204
+    Luts                     : 926
+    Power                    : 3.1429999999999998
+    Registers                : 680
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.4790000000000001
+    Design slack             : 0.52099999999999991
+    Frequency                : 287.43891922966367
+    AreaxTime                : 5208486.0881480007
+    Time                     : 5624.7149980000004
+    Tot. Time                : 5624.7149980000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Starting execution of HLS::Evaluation
+    Total cycles             : 2524952 cycles
+    Number of executions     : 1
+    Average execution        : 2524952 cycles
+    Slices                   : 213
+    Luts                     : 957
+    Power                    : 3.1419999999999999
+    Registers                : 682
+    DSPs                     : 2
+    BRAMs                    : 0
+    Clock period             : 4
+    Design minimum period    : 3.5939999999999999
+    Design slack             : 0.40600000000000014
+    Frequency                : 278.24151363383419
+    AreaxTime                : 8684466.3560159989
+    Time                     : 9074.6774879999994
+    Tot. Time                : 9074.6774879999994</t>
+  </si>
+  <si>
+    <t>verilator error</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1777,7 +1897,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2092,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H3" sqref="H3:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2106,14 +2225,16 @@
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" customWidth="1"/>
     <col min="7" max="7" width="24" style="4" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2135,14 +2256,14 @@
       <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -2164,12 +2285,14 @@
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -2191,12 +2314,14 @@
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2218,12 +2343,14 @@
       <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2245,12 +2372,14 @@
       <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2272,12 +2401,14 @@
       <c r="G8" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I8" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -2299,10 +2430,12 @@
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2311,10 +2444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4718C2A3-79B5-2E49-96DF-E5F4ED4798BE}">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,10 +2522,10 @@
       <c r="E4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>63</v>
       </c>
       <c r="H4" s="6">
@@ -2490,7 +2623,7 @@
       <c r="E7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -3893,13 +4026,16 @@
         <v>11</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F57" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H57" s="6">
+        <v>29297</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3914,13 +4050,16 @@
         <v>11</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H58" s="6">
+        <v>26687</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3935,13 +4074,16 @@
         <v>11</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H59" s="6">
+        <v>25457</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3956,13 +4098,16 @@
         <v>11</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H60" s="6">
+        <v>26537</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3977,13 +4122,16 @@
         <v>11</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>80</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H61" s="6">
+        <v>16097</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3998,13 +4146,16 @@
         <v>11</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>78</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H62" s="6">
+        <v>10097</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4019,13 +4170,16 @@
         <v>11</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="H63" s="6">
+        <v>7157</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4040,37 +4194,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>87</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="H64" s="6">
+        <v>5687</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
-      <c r="C65" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>43</v>
       </c>
@@ -4082,16 +4226,19 @@
         <v>16</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>111</v>
+        <v>223</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="H66" s="6">
+        <v>116192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>43</v>
       </c>
@@ -4103,16 +4250,19 @@
         <v>16</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="H67" s="6">
+        <v>61892</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>43</v>
       </c>
@@ -4124,16 +4274,19 @@
         <v>16</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="H68" s="6">
+        <v>38612</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>43</v>
       </c>
@@ -4145,13 +4298,40 @@
         <v>16</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F69" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="H69" s="6">
+        <v>27332</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="6" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G69" s="7" t="s">
-        <v>226</v>
+      <c r="G70" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="H70" s="6">
+        <v>21692</v>
       </c>
     </row>
   </sheetData>
@@ -4397,7 +4577,7 @@
       <c r="I11">
         <v>93705</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4429,7 +4609,7 @@
       <c r="I12">
         <v>301800</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4461,7 +4641,7 @@
       <c r="I13">
         <v>1064580</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4493,7 +4673,7 @@
       <c r="I14">
         <v>2298510</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4525,7 +4705,7 @@
       <c r="I15">
         <v>3987840</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4557,7 +4737,7 @@
       <c r="I16">
         <v>6136470</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4712,7 +4892,7 @@
       <c r="G25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4735,7 +4915,7 @@
       <c r="G26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4758,7 +4938,7 @@
       <c r="G27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="K27" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4781,7 +4961,7 @@
       <c r="G28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" t="s">
         <v>204</v>
       </c>
     </row>
@@ -4804,7 +4984,7 @@
       <c r="G29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4827,7 +5007,7 @@
       <c r="G30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="K30" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4855,7 +5035,7 @@
       <c r="G32" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K32" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4878,7 +5058,7 @@
       <c r="G33" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K33" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4901,7 +5081,7 @@
       <c r="G34" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="K34" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4924,7 +5104,7 @@
       <c r="G35" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4947,7 +5127,7 @@
       <c r="G36" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K36" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4970,7 +5150,7 @@
       <c r="G37" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K37" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4978,7 +5158,6 @@
       <c r="A38" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -4999,7 +5178,7 @@
       <c r="G39" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K39" s="12" t="s">
+      <c r="K39" t="s">
         <v>210</v>
       </c>
     </row>
@@ -5022,7 +5201,7 @@
       <c r="G40" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="K40" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5045,7 +5224,7 @@
       <c r="G41" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="K41" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5068,7 +5247,7 @@
       <c r="G42" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="K42" t="s">
         <v>217</v>
       </c>
     </row>
@@ -5091,7 +5270,7 @@
       <c r="G43" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="K43" t="s">
         <v>219</v>
       </c>
     </row>
@@ -5114,7 +5293,7 @@
       <c r="G44" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="K44" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>